<commit_message>
New data, updated figures, breakthrough-infections and a bunch of other stuff
</commit_message>
<xml_diff>
--- a/DanskeData/gennembrud.xlsx
+++ b/DanskeData/gennembrud.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4915,7 +4916,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5357,7 +5358,7 @@
         <v>11753</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:F13" si="3">SUM(C2:C12)</f>
+        <f t="shared" ref="C13:D13" si="3">SUM(C2:C12)</f>
         <v>1583</v>
       </c>
       <c r="D13">

</xml_diff>